<commit_message>
feat: implement persistent file upload handling and data directory structure
</commit_message>
<xml_diff>
--- a/excel_ocr/output/financial_statements_from_gpt.xlsx
+++ b/excel_ocr/output/financial_statements_from_gpt.xlsx
@@ -9,22 +9,21 @@
   <sheets>
     <sheet name="Balance Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Income Statement" sheetId="2" r:id="rId2"/>
-    <sheet name="Cash Flow Statement" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t xml:space="preserve"> Indicator</t>
   </si>
   <si>
-    <t>Current Year (2025)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Previous Year (2024)* </t>
+    <t>Current Year (2024)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous Year (2023) </t>
   </si>
   <si>
     <t xml:space="preserve"> Cash and Cash Equivalents</t>
@@ -33,58 +32,100 @@
     <t xml:space="preserve"> Accounts Receivable</t>
   </si>
   <si>
+    <t xml:space="preserve"> Property, Plant and Equipment</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Total Assets</t>
   </si>
   <si>
     <t xml:space="preserve"> Accounts Payable</t>
   </si>
   <si>
-    <t xml:space="preserve"> Total Liabilities</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Total Equity</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Total Liabilities and Equity</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>6,000</t>
-  </si>
-  <si>
-    <t>6,500</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0                     </t>
+    <t xml:space="preserve"> Retained Earnings</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Equity &amp; Liabilities</t>
+  </si>
+  <si>
+    <t>1,000</t>
+  </si>
+  <si>
+    <t>11,987,605.97</t>
+  </si>
+  <si>
+    <t>3,489,523.92</t>
+  </si>
+  <si>
+    <t>14,355,193.96</t>
+  </si>
+  <si>
+    <t>-12,443,892.15</t>
+  </si>
+  <si>
+    <t>-2,444,853.69</t>
+  </si>
+  <si>
+    <t>-14,888,745.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,000                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,711,454.12        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,494,523.92         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,424,369.47        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10,979,515.78       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2,741,596.38        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,721,112.16        </t>
   </si>
   <si>
     <t xml:space="preserve"> Revenue</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cost of Goods Sold</t>
+    <t xml:space="preserve"> Cost of Goods Sold (COGS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> General and Administrative Expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Profit Before Tax</t>
   </si>
   <si>
     <t xml:space="preserve"> Net Profit</t>
   </si>
   <si>
-    <t>12,000</t>
-  </si>
-  <si>
-    <t>4,500</t>
-  </si>
-  <si>
-    <t>7,500</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Net Change in Cash</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cash Flow from Operating Activities</t>
+    <t>-1,276,151.85</t>
+  </si>
+  <si>
+    <t>-367,148.33</t>
+  </si>
+  <si>
+    <t>937,434.64</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,727,145.61        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-428,513.69          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,105,786.47         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A                  </t>
   </si>
 </sst>
 </file>
@@ -467,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -478,7 +519,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -489,7 +530,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -500,7 +541,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -508,10 +549,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -519,10 +560,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -530,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -543,7 +584,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -562,81 +603,57 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: integrate Google Cloud Storage for file uploads, downloads, and deletion; update requirements and Docker script
</commit_message>
<xml_diff>
--- a/excel_ocr/output/financial_statements_from_gpt.xlsx
+++ b/excel_ocr/output/financial_statements_from_gpt.xlsx
@@ -9,21 +9,22 @@
   <sheets>
     <sheet name="Balance Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Income Statement" sheetId="2" r:id="rId2"/>
+    <sheet name="Cash Flow Statement" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
-  <si>
-    <t xml:space="preserve"> Indicator</t>
-  </si>
-  <si>
-    <t>Current Year (2024)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Previous Year (2023) </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+  <si>
+    <t xml:space="preserve"> **Balance Sheet Indicators**</t>
+  </si>
+  <si>
+    <t>**Current Year (2024)**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Previous Year (2023)** </t>
   </si>
   <si>
     <t xml:space="preserve"> Cash and Cash Equivalents</t>
@@ -32,7 +33,7 @@
     <t xml:space="preserve"> Accounts Receivable</t>
   </si>
   <si>
-    <t xml:space="preserve"> Property, Plant and Equipment</t>
+    <t xml:space="preserve"> Property, Plant and Equipment (Net)</t>
   </si>
   <si>
     <t xml:space="preserve"> Total Assets</t>
@@ -41,19 +42,19 @@
     <t xml:space="preserve"> Accounts Payable</t>
   </si>
   <si>
-    <t xml:space="preserve"> Retained Earnings</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Total Equity &amp; Liabilities</t>
-  </si>
-  <si>
-    <t>1,000</t>
+    <t xml:space="preserve"> Accumulated Profit/(Loss)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Liabilities</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
   <si>
     <t>11,987,605.97</t>
   </si>
   <si>
-    <t>3,489,523.92</t>
+    <t>3,494,523.92</t>
   </si>
   <si>
     <t>14,355,193.96</t>
@@ -68,64 +69,88 @@
     <t>-14,888,745.84</t>
   </si>
   <si>
-    <t xml:space="preserve">1,000                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,711,454.12        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,494,523.92         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,424,369.47        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-10,979,515.78       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,741,596.38        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,721,112.16        </t>
+    <t xml:space="preserve">1000                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,711,454.12            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,494,523.92             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,424,369.47            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10,979,515.78           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2,741,596.38            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13,721,112.16           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> **Income Statement Indicators**</t>
   </si>
   <si>
     <t xml:space="preserve"> Revenue</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cost of Goods Sold (COGS)</t>
+    <t xml:space="preserve"> Cost of Goods Sold</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gross Profit</t>
   </si>
   <si>
     <t xml:space="preserve"> General and Administrative Expenses</t>
   </si>
   <si>
-    <t xml:space="preserve"> Profit Before Tax</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Net Profit</t>
   </si>
   <si>
     <t>-1,276,151.85</t>
   </si>
   <si>
-    <t>-367,148.33</t>
-  </si>
-  <si>
-    <t>937,434.64</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,727,145.61        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">-428,513.69          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,105,786.47         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A                  </t>
+    <t>367,148.33</t>
+  </si>
+  <si>
+    <t>*N/A*</t>
+  </si>
+  <si>
+    <t>*Consolidated within Expense Total*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,727,145.61            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">428,073.69               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">*N/A*                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Consolidated within Expense Total* </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> **Cash Flow Indicators**</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Depreciation and Amortization</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Cash Flow</t>
+  </si>
+  <si>
+    <t>350,277.36</t>
+  </si>
+  <si>
+    <t>533,551.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">349,452.36               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">296,742.69               </t>
   </si>
 </sst>
 </file>
@@ -592,7 +617,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -603,57 +628,103 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>